<commit_message>
removing geographic data that we don't use
</commit_message>
<xml_diff>
--- a/data/RCT wave 3/Raw/Wave 3 IDs for missing respondents_5Oct2022.xlsx
+++ b/data/RCT wave 3/Raw/Wave 3 IDs for missing respondents_5Oct2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/879b7e2da8cffd9d/Female_transport_Riyadh/Surveys and data/RCT wave 3/Raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prodduke-my.sharepoint.com/personal/kms110_duke_edu/Documents/saudi_women_driving/data/RCT wave 3/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77209A60-D1D1-104A-9FD7-790104F9D6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{77209A60-D1D1-104A-9FD7-790104F9D6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB0CEB6B-2079-624F-A157-F0DDE00E4A9D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{EE464CD2-BCC3-164E-8E5E-CD45438D994A}"/>
+    <workbookView xWindow="33320" yWindow="-4920" windowWidth="28800" windowHeight="16260" xr2:uid="{EE464CD2-BCC3-164E-8E5E-CD45438D994A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>IP Address</t>
-  </si>
-  <si>
-    <t>188.53.170.116</t>
-  </si>
-  <si>
-    <t>93.169.151.135</t>
-  </si>
-  <si>
-    <t>77.232.122.142</t>
-  </si>
-  <si>
-    <t>77.232.122.168</t>
-  </si>
-  <si>
-    <t>51.36.4.177</t>
-  </si>
-  <si>
-    <t>77.232.122.123</t>
   </si>
   <si>
     <t>StartDate</t>
@@ -143,9 +125,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -183,7 +165,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -289,7 +271,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -431,7 +413,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,9 +423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25741E16-443D-F040-8984-192E389D6521}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -456,25 +436,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -487,9 +467,6 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
       <c r="E2">
         <v>100</v>
       </c>
@@ -510,9 +487,6 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
       <c r="E3">
         <v>100</v>
       </c>
@@ -533,9 +507,6 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
       <c r="E4">
         <v>100</v>
       </c>
@@ -556,9 +527,6 @@
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
       <c r="E5">
         <v>100</v>
       </c>
@@ -579,9 +547,6 @@
       <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
       <c r="E6">
         <v>100</v>
       </c>
@@ -602,9 +567,6 @@
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
       <c r="E7">
         <v>100</v>
       </c>
@@ -625,9 +587,6 @@
       <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
       <c r="E8">
         <v>100</v>
       </c>
@@ -648,9 +607,6 @@
       <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
       <c r="E9">
         <v>100</v>
       </c>
@@ -671,9 +627,6 @@
       <c r="C10" t="s">
         <v>0</v>
       </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
       <c r="E10">
         <v>100</v>
       </c>
@@ -694,9 +647,6 @@
       <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
       <c r="E11">
         <v>100</v>
       </c>
@@ -717,9 +667,6 @@
       <c r="C12" t="s">
         <v>0</v>
       </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
       <c r="E12">
         <v>100</v>
       </c>
@@ -740,9 +687,6 @@
       <c r="C13" t="s">
         <v>0</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
       <c r="E13">
         <v>100</v>
       </c>
@@ -762,9 +706,6 @@
       </c>
       <c r="C14" t="s">
         <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
       </c>
       <c r="E14">
         <v>100</v>

</xml_diff>